<commit_message>
Speaker Driver complete, report updated
</commit_message>
<xml_diff>
--- a/assignments/per_1_speaker_driver/tables.xlsx
+++ b/assignments/per_1_speaker_driver/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisg\Desktop\Winter 2018\CPE-233\assignments\per_1_speaker_driver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F9B25F-45D2-4650-B496-7C6CEAFBF6F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97817922-075F-423C-88A8-E41F86ACC853}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8040" xr2:uid="{3A8B29BC-26CD-4FC7-9009-A457400A334B}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
   <si>
     <t>Input Value</t>
   </si>
@@ -41,9 +40,6 @@
   </si>
   <si>
     <t>Octave</t>
-  </si>
-  <si>
-    <t>Hz</t>
   </si>
   <si>
     <t>none</t>
@@ -116,12 +112,25 @@
       <t>)</t>
     </r>
   </si>
+  <si>
+    <t>% error</t>
+  </si>
+  <si>
+    <t>Verification (Hz)</t>
+  </si>
+  <si>
+    <t>Frequency (Hz)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.00000%"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,8 +146,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,6 +193,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -182,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -197,6 +233,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -513,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC782DA-2900-42F4-9FCE-84B7A2F4F5BD}">
-  <dimension ref="B2:H39"/>
+  <dimension ref="B2:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,12 +584,13 @@
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -540,24 +601,30 @@
         <v>2</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -565,16 +632,22 @@
       <c r="F3" s="2">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G3" s="13">
+        <v>0</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2">
         <v>6</v>
@@ -586,13 +659,20 @@
         <f>ROUND(((100000000)/(2*E4)),0)</f>
         <v>47778</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="13">
+        <v>1046.5999999999999</v>
+      </c>
+      <c r="H4" s="10">
+        <f xml:space="preserve"> ABS((E4-G4)/E4)</f>
+        <v>9.3645305981217755E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2">
         <v>6</v>
@@ -604,13 +684,20 @@
         <f t="shared" ref="F5:F39" si="0">ROUND(((100000000)/(2*E5)),0)</f>
         <v>45097</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="13">
+        <v>1108.7</v>
+      </c>
+      <c r="H5" s="10">
+        <f t="shared" ref="H5:H39" si="1" xml:space="preserve"> ABS((E5-G5)/E5)</f>
+        <v>2.7959892886506347E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2">
         <v>6</v>
@@ -622,13 +709,20 @@
         <f t="shared" si="0"/>
         <v>42566</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="13">
+        <v>1174.7</v>
+      </c>
+      <c r="H6" s="10">
+        <f t="shared" si="1"/>
+        <v>3.490374653404943E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2">
         <v>6</v>
@@ -640,13 +734,20 @@
         <f t="shared" si="0"/>
         <v>40177</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G7" s="13">
+        <v>1244.5</v>
+      </c>
+      <c r="H7" s="10">
+        <f t="shared" si="1"/>
+        <v>6.4282431290423192E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="2">
         <v>6</v>
@@ -658,13 +759,20 @@
         <f t="shared" si="0"/>
         <v>37922</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G8" s="13">
+        <v>1318.6</v>
+      </c>
+      <c r="H8" s="10">
+        <f t="shared" si="1"/>
+        <v>6.8258867964534321E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="2">
         <v>6</v>
@@ -676,13 +784,20 @@
         <f t="shared" si="0"/>
         <v>35793</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G9" s="13">
+        <v>1397</v>
+      </c>
+      <c r="H9" s="10">
+        <f t="shared" si="1"/>
+        <v>6.2280184950665562E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="2">
         <v>6</v>
@@ -694,13 +809,20 @@
         <f t="shared" si="0"/>
         <v>33784</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="13">
+        <v>1480</v>
+      </c>
+      <c r="H10" s="10">
+        <f t="shared" si="1"/>
+        <v>1.4865085832312721E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="2">
         <v>6</v>
@@ -712,13 +834,20 @@
         <f t="shared" si="0"/>
         <v>31888</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="13">
+        <v>1568</v>
+      </c>
+      <c r="H11" s="10">
+        <f t="shared" si="1"/>
+        <v>1.1479723619294803E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="2">
         <v>6</v>
@@ -730,13 +859,20 @@
         <f t="shared" si="0"/>
         <v>30098</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G12" s="13">
+        <v>1661.4</v>
+      </c>
+      <c r="H12" s="10">
+        <f t="shared" si="1"/>
+        <v>1.0895613401968073E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="2">
         <v>6</v>
@@ -748,13 +884,20 @@
         <f t="shared" si="0"/>
         <v>28409</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G13" s="13">
+        <v>1760.1</v>
+      </c>
+      <c r="H13" s="10">
+        <f t="shared" si="1"/>
+        <v>5.6818181818130142E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>11</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="2">
         <v>6</v>
@@ -766,13 +909,20 @@
         <f t="shared" si="0"/>
         <v>26815</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G14" s="13">
+        <v>1864.6</v>
+      </c>
+      <c r="H14" s="10">
+        <f t="shared" si="1"/>
+        <v>2.9496073000133357E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="2">
         <v>6</v>
@@ -784,13 +934,20 @@
         <f t="shared" si="0"/>
         <v>25310</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G15" s="13">
+        <v>1975.5</v>
+      </c>
+      <c r="H15" s="10">
+        <f t="shared" si="1"/>
+        <v>1.6704352698690316E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>13</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="3">
         <v>7</v>
@@ -803,13 +960,20 @@
         <f t="shared" si="0"/>
         <v>23889</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="7">
+        <v>2093.1</v>
+      </c>
+      <c r="H16" s="11">
+        <f t="shared" si="1"/>
+        <v>4.5867088643883934E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17" s="3">
         <v>7</v>
@@ -822,13 +986,20 @@
         <f t="shared" si="0"/>
         <v>22548</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="7">
+        <v>2217.5</v>
+      </c>
+      <c r="H17" s="11">
+        <f t="shared" si="1"/>
+        <v>1.7136708543375678E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="3">
         <v>7</v>
@@ -841,184 +1012,254 @@
         <f t="shared" si="0"/>
         <v>21283</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="7">
+        <v>2349.4</v>
+      </c>
+      <c r="H18" s="11">
+        <f t="shared" si="1"/>
+        <v>3.490374653404943E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <v>16</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D19" s="3">
         <v>7</v>
       </c>
       <c r="E19" s="3">
-        <f t="shared" ref="E19:E27" si="1">E7*2</f>
+        <f t="shared" ref="E19:E27" si="2">E7*2</f>
         <v>2489.0160000000001</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="0"/>
         <v>20088</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="7">
+        <v>2489</v>
+      </c>
+      <c r="H19" s="11">
+        <f t="shared" si="1"/>
+        <v>6.4282431290423192E-6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" s="3">
         <v>7</v>
       </c>
       <c r="E20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2637.02</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="0"/>
         <v>18961</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="7">
+        <v>2637</v>
+      </c>
+      <c r="H20" s="11">
+        <f t="shared" si="1"/>
+        <v>7.5843186627260357E-6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" s="3">
         <v>7</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2793.826</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="0"/>
         <v>17897</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="7">
+        <v>2793.9</v>
+      </c>
+      <c r="H21" s="11">
+        <f t="shared" si="1"/>
+        <v>2.648697520893181E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>19</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D22" s="3">
         <v>7</v>
       </c>
       <c r="E22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2959.9560000000001</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="0"/>
         <v>16892</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="7">
+        <v>2960</v>
+      </c>
+      <c r="H22" s="11">
+        <f t="shared" si="1"/>
+        <v>1.4865085832312721E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <v>20</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23" s="3">
         <v>7</v>
       </c>
       <c r="E23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3135.9639999999999</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="0"/>
         <v>15944</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="7">
+        <v>3136</v>
+      </c>
+      <c r="H23" s="11">
+        <f t="shared" si="1"/>
+        <v>1.1479723619294803E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <v>21</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D24" s="3">
         <v>7</v>
       </c>
       <c r="E24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3322.4380000000001</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="0"/>
         <v>15049</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="7">
+        <v>3322.4</v>
+      </c>
+      <c r="H24" s="11">
+        <f t="shared" si="1"/>
+        <v>1.1437384234110889E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <v>22</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D25" s="3">
         <v>7</v>
       </c>
       <c r="E25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3520</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="0"/>
         <v>14205</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="7">
+        <v>3520.1</v>
+      </c>
+      <c r="H25" s="11">
+        <f t="shared" si="1"/>
+        <v>2.8409090909065071E-5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <v>23</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D26" s="3">
         <v>7</v>
       </c>
       <c r="E26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3729.31</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="0"/>
         <v>13407</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="7">
+        <v>3729.5</v>
+      </c>
+      <c r="H26" s="11">
+        <f t="shared" si="1"/>
+        <v>5.0947762454731457E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <v>24</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D27" s="3">
         <v>7</v>
       </c>
       <c r="E27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3951.0659999999998</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="0"/>
         <v>12655</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="7">
+        <v>3951.1</v>
+      </c>
+      <c r="H27" s="11">
+        <f t="shared" si="1"/>
+        <v>8.6052726024079335E-6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="4">
         <v>25</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D28" s="4">
         <v>8</v>
@@ -1031,13 +1272,20 @@
         <f t="shared" si="0"/>
         <v>11945</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="8">
+        <v>4186.2</v>
+      </c>
+      <c r="H28" s="12">
+        <f t="shared" si="1"/>
+        <v>4.5867088643883934E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
         <v>26</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D29" s="4">
         <v>8</v>
@@ -1050,195 +1298,272 @@
         <f t="shared" si="0"/>
         <v>11274</v>
       </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="8">
+        <v>4435</v>
+      </c>
+      <c r="H29" s="12">
+        <f t="shared" si="1"/>
+        <v>1.7136708543375678E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="4">
         <v>27</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D30" s="4">
         <v>8</v>
       </c>
       <c r="E30" s="4">
-        <f t="shared" ref="E30:E39" si="2">E18*2</f>
+        <f t="shared" ref="E30:E39" si="3">E18*2</f>
         <v>4698.6360000000004</v>
       </c>
       <c r="F30" s="4">
         <f t="shared" si="0"/>
         <v>10641</v>
       </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="8">
+        <v>4698.7</v>
+      </c>
+      <c r="H30" s="12">
+        <f t="shared" si="1"/>
+        <v>1.3620974257081436E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
         <v>28</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D31" s="4">
         <v>8</v>
       </c>
       <c r="E31" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4978.0320000000002</v>
       </c>
       <c r="F31" s="4">
         <f t="shared" si="0"/>
         <v>10044</v>
       </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="8">
+        <v>4978.1000000000004</v>
+      </c>
+      <c r="H31" s="12">
+        <f t="shared" si="1"/>
+        <v>1.366001664919209E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="4">
         <v>29</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D32" s="4">
         <v>8</v>
       </c>
       <c r="E32" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5274.04</v>
       </c>
       <c r="F32" s="4">
         <f t="shared" si="0"/>
         <v>9480</v>
       </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="8">
+        <v>5274.3</v>
+      </c>
+      <c r="H32" s="12">
+        <f t="shared" si="1"/>
+        <v>4.9298071307805453E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="4">
         <v>30</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D33" s="4">
         <v>8</v>
       </c>
       <c r="E33" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5587.652</v>
       </c>
       <c r="F33" s="4">
         <f t="shared" si="0"/>
         <v>8948</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="8">
+        <v>5587.8</v>
+      </c>
+      <c r="H33" s="12">
+        <f t="shared" si="1"/>
+        <v>2.648697520893181E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="4">
         <v>31</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D34" s="4">
         <v>8</v>
       </c>
       <c r="E34" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5919.9120000000003</v>
       </c>
       <c r="F34" s="4">
         <f t="shared" si="0"/>
         <v>8446</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="8">
+        <v>5920</v>
+      </c>
+      <c r="H34" s="12">
+        <f t="shared" si="1"/>
+        <v>1.4865085832312721E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="4">
         <v>32</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D35" s="4">
         <v>8</v>
       </c>
       <c r="E35" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6271.9279999999999</v>
       </c>
       <c r="F35" s="4">
         <f t="shared" si="0"/>
         <v>7972</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="8">
+        <v>6272</v>
+      </c>
+      <c r="H35" s="12">
+        <f t="shared" si="1"/>
+        <v>1.1479723619294803E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="4">
         <v>33</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D36" s="4">
         <v>8</v>
       </c>
       <c r="E36" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6644.8760000000002</v>
       </c>
       <c r="F36" s="4">
         <f t="shared" si="0"/>
         <v>7525</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="8">
+        <v>6645.4</v>
+      </c>
+      <c r="H36" s="12">
+        <f t="shared" si="1"/>
+        <v>7.8857754456130173E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="4">
         <v>34</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D37" s="4">
         <v>8</v>
       </c>
       <c r="E37" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7040</v>
       </c>
       <c r="F37" s="4">
         <f t="shared" si="0"/>
         <v>7102</v>
       </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="8">
+        <v>7040.3</v>
+      </c>
+      <c r="H37" s="12">
+        <f t="shared" si="1"/>
+        <v>4.2613636363662205E-5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="4">
         <v>35</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D38" s="4">
         <v>8</v>
       </c>
       <c r="E38" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7458.62</v>
       </c>
       <c r="F38" s="4">
         <f t="shared" si="0"/>
         <v>6704</v>
       </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="8">
+        <v>7459.6</v>
+      </c>
+      <c r="H38" s="12">
+        <f t="shared" si="1"/>
+        <v>1.3139159790959628E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="4">
         <v>36</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D39" s="4">
         <v>8</v>
       </c>
       <c r="E39" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7902.1319999999996</v>
       </c>
       <c r="F39" s="4">
         <f t="shared" si="0"/>
         <v>6327</v>
+      </c>
+      <c r="G39" s="8">
+        <v>7902.9</v>
+      </c>
+      <c r="H39" s="12">
+        <f t="shared" si="1"/>
+        <v>9.7188961156309347E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>